<commit_message>
refactoring. all tests passing
</commit_message>
<xml_diff>
--- a/tests/resources/spent_data_master_2_2020.xlsx
+++ b/tests/resources/spent_data_master_2_2020.xlsx
@@ -127,7 +127,7 @@
     <t xml:space="preserve">Pre 19-20 BL Income both Revenue and Capital</t>
   </si>
   <si>
-    <t xml:space="preserve">Pre 19-20 CDEL Forecast Total</t>
+    <t xml:space="preserve">Pre-profile CDEL Forecast one off new costs</t>
   </si>
   <si>
     <t xml:space="preserve">Pre 19-20 CDEL Forecast recurring new costs</t>
@@ -136,7 +136,7 @@
     <t xml:space="preserve">Pre 19-20 CDEL Forecast recurring old costs</t>
   </si>
   <si>
-    <t xml:space="preserve">Pre 19-20 Forecast Non-Gov</t>
+    <t xml:space="preserve">Pre-profile Forecast Non-Gov</t>
   </si>
   <si>
     <t xml:space="preserve">Pre-profile CDEL</t>
@@ -236,12 +236,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -264,13 +268,13 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B37" activeCellId="0" sqref="B37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C39" activeCellId="0" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="2" style="0" width="29.21"/>
   </cols>
   <sheetData>
@@ -722,15 +726,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="s">
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="0" t="n">
         <v>0</v>
       </c>
       <c r="C33" s="0" t="n">
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="D33" s="0" t="n">
         <v>0</v>

</xml_diff>